<commit_message>
Adicionados Diagramas de Sequência relativos aos Use Cases do Tiago e Cesário, alterações de promenores em algumas especificações
</commit_message>
<xml_diff>
--- a/Fase2/UML/Especificação de Use Cases/Ver avaliações.xlsx
+++ b/Fase2/UML/Especificação de Use Cases/Ver avaliações.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\OneDrive\Documents\GitHub\li4-17-18\Fase2\UML\Especificação de Use Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF916F5D-DF7A-4180-95DB-85A4A373462A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF86BEDB-6315-4A95-A4E1-B4D561B5F7AC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" xr2:uid="{29E41BAE-F072-473F-BDD1-50B5F439C3F0}"/>
   </bookViews>
@@ -109,10 +109,10 @@
     <t xml:space="preserve">Pintor devidamente autenticado </t>
   </si>
   <si>
-    <t>Apresenta todos as Avaliações dos todos os seus serviços</t>
-  </si>
-  <si>
     <t>Indica que pretende ver as avaliações dos seus serviços</t>
+  </si>
+  <si>
+    <t>Apresenta todos as Avaliações de todos os seus serviços</t>
   </si>
 </sst>
 </file>
@@ -500,7 +500,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +579,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -590,7 +590,7 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Alteradas Irregularidades em diagramas anteriores
</commit_message>
<xml_diff>
--- a/Fase2/UML/Especificação de Use Cases/Ver avaliações.xlsx
+++ b/Fase2/UML/Especificação de Use Cases/Ver avaliações.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\OneDrive\Documents\GitHub\li4-17-18\Fase2\UML\Especificação de Use Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF86BEDB-6315-4A95-A4E1-B4D561B5F7AC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82191189-3BA6-4A49-9D31-F33C17F1B1CB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" xr2:uid="{29E41BAE-F072-473F-BDD1-50B5F439C3F0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -112,7 +112,13 @@
     <t>Indica que pretende ver as avaliações dos seus serviços</t>
   </si>
   <si>
-    <t>Apresenta todos as Avaliações de todos os seus serviços</t>
+    <t>Apresenta lista de Serviços efectuados</t>
+  </si>
+  <si>
+    <t>Escolhe Serviço</t>
+  </si>
+  <si>
+    <t>Apresenta Avaliação</t>
   </si>
 </sst>
 </file>
@@ -500,7 +506,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,15 +601,23 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1">
+        <v>4</v>
+      </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>

</xml_diff>